<commit_message>
OpenAi response Data cleaning
OpenAi response training
</commit_message>
<xml_diff>
--- a/Data/AICustomerData.xlsx
+++ b/Data/AICustomerData.xlsx
@@ -37,7 +37,7 @@
     <x:t>Ai Generated Sub Categories</x:t>
   </x:si>
   <x:si>
-    <x:t>CS2025_00051</x:t>
+    <x:t>CS2025_00142</x:t>
   </x:si>
   <x:si>
     <x:t>Alice</x:t>
@@ -52,10 +52,10 @@
     <x:t xml:space="preserve"> Unable to log in to my account after recent update.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Account Access."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00052</x:t>
+    <x:t>Authentication Issue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00143</x:t>
   </x:si>
   <x:si>
     <x:t>Amanda</x:t>
@@ -67,10 +67,10 @@
     <x:t xml:space="preserve"> I am getting frequent error messages on the desktop application.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Software Troubleshooting."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00053</x:t>
+    <x:t>Software Troubleshooting.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00144</x:t>
   </x:si>
   <x:si>
     <x:t>Benjamin</x:t>
@@ -85,10 +85,10 @@
     <x:t xml:space="preserve"> I was charged for a subscription I canceled last month.</x:t>
   </x:si>
   <x:si>
-    <x:t>Subcategory Suggestion: Refund Request</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00054</x:t>
+    <x:t>Refund Request</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00145</x:t>
   </x:si>
   <x:si>
     <x:t>Bob</x:t>
@@ -100,10 +100,10 @@
     <x:t xml:space="preserve"> Incorrect charge appeared on my credit card statement.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Credit Card"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00055</x:t>
+    <x:t>Payment Disputes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00146</x:t>
   </x:si>
   <x:si>
     <x:t>Catherine</x:t>
@@ -118,10 +118,10 @@
     <x:t xml:space="preserve"> What security features are included in your software?</x:t>
   </x:si>
   <x:si>
-    <x:t>Authentication Methods</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00056</x:t>
+    <x:t>Product Features.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00147</x:t>
   </x:si>
   <x:si>
     <x:t>Clara</x:t>
@@ -133,10 +133,10 @@
     <x:t xml:space="preserve"> Do you offer discounts for bulk purchases?</x:t>
   </x:si>
   <x:si>
-    <x:t>Subcategory Suggestion: Pricing Options</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00057</x:t>
+    <x:t>Product Pricing.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00148</x:t>
   </x:si>
   <x:si>
     <x:t>Daniel</x:t>
@@ -148,10 +148,10 @@
     <x:t xml:space="preserve"> The system doesn't recognize my external hard drive.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Hardware Troubleshooting."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00058</x:t>
+    <x:t>Hardware Issue.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00149</x:t>
   </x:si>
   <x:si>
     <x:t>David</x:t>
@@ -163,10 +163,10 @@
     <x:t xml:space="preserve"> Website shows a 404 error when trying to access the support page.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Website Maintenance."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00059</x:t>
+    <x:t>Website Maintenance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00150</x:t>
   </x:si>
   <x:si>
     <x:t>Emma</x:t>
@@ -178,10 +178,10 @@
     <x:t xml:space="preserve"> I need a copy of my last three invoices for reimbursement purposes.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Document Retrieval."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00060</x:t>
+    <x:t>Invoice Request.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00151</x:t>
   </x:si>
   <x:si>
     <x:t>Frank</x:t>
@@ -193,10 +193,10 @@
     <x:t xml:space="preserve"> What are your customer service operating hours?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Operating Hours"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00061</x:t>
+    <x:t>Operating Hours</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00152</x:t>
   </x:si>
   <x:si>
     <x:t>Grace</x:t>
@@ -208,10 +208,10 @@
     <x:t xml:space="preserve"> My mobile app keeps crashing whenever I try to open the settings page.</x:t>
   </x:si>
   <x:si>
-    <x:t>"App Performance"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00062</x:t>
+    <x:t>App Troubleshooting.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00153</x:t>
   </x:si>
   <x:si>
     <x:t>Harry</x:t>
@@ -223,10 +223,7 @@
     <x:t xml:space="preserve"> I accidentally made a duplicate payment. Can I get a refund?</x:t>
   </x:si>
   <x:si>
-    <x:t>Refund Request</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00063</x:t>
+    <x:t>CS2025_00154</x:t>
   </x:si>
   <x:si>
     <x:t>Isabella</x:t>
@@ -238,10 +235,10 @@
     <x:t xml:space="preserve"> Can I change my subscription plan mid-cycle without penalties?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Billing Information"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00064</x:t>
+    <x:t>Billing Inquiry.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00155</x:t>
   </x:si>
   <x:si>
     <x:t>Jack</x:t>
@@ -253,10 +250,10 @@
     <x:t xml:space="preserve"> I am experiencing connectivity issues with your cloud service.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Network Troubleshooting."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00065</x:t>
+    <x:t>Network Troubleshooting.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00156</x:t>
   </x:si>
   <x:si>
     <x:t>Karen</x:t>
@@ -268,10 +265,10 @@
     <x:t xml:space="preserve"> My subscription renewal failed, and my account is deactivated.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Account Management"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00066</x:t>
+    <x:t>Account Management</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00157</x:t>
   </x:si>
   <x:si>
     <x:t>Liam</x:t>
@@ -283,10 +280,10 @@
     <x:t xml:space="preserve"> The software update failed to install on my device.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Software Installation."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00067</x:t>
+    <x:t>Software Installation.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00158</x:t>
   </x:si>
   <x:si>
     <x:t>Mia</x:t>
@@ -298,10 +295,10 @@
     <x:t xml:space="preserve"> Do you have a physical store near my location?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Store Locator"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00068</x:t>
+    <x:t>Store Location.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00159</x:t>
   </x:si>
   <x:si>
     <x:t>Noah</x:t>
@@ -313,10 +310,10 @@
     <x:t xml:space="preserve"> I need help configuring my email on a new device.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Email Setup."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00069</x:t>
+    <x:t>Email Setup.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00160</x:t>
   </x:si>
   <x:si>
     <x:t>Olivia</x:t>
@@ -328,10 +325,10 @@
     <x:t xml:space="preserve"> Can I split my annual payment into monthly installments?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Payment Plans"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00070</x:t>
+    <x:t>Payment Plans.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00161</x:t>
   </x:si>
   <x:si>
     <x:t>Paul</x:t>
@@ -343,10 +340,10 @@
     <x:t xml:space="preserve"> I am unable to reset my password due to an error.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Password Reset"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00071</x:t>
+    <x:t>Password Reset</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00162</x:t>
   </x:si>
   <x:si>
     <x:t>Quinn</x:t>
@@ -358,10 +355,10 @@
     <x:t xml:space="preserve"> Can you explain the differences between your plans?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Plan Comparison."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00072</x:t>
+    <x:t>Product Comparison.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00163</x:t>
   </x:si>
   <x:si>
     <x:t>Rachel</x:t>
@@ -373,25 +370,10 @@
     <x:t xml:space="preserve"> Why was I charged twice for the same transaction?</x:t>
   </x:si>
   <x:si>
-    <x:t>Subcategory Suggestion: Payment Issue</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00073</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alice Johnson</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Technical Support</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Unable to log in to the website.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>"Login Issues."</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00074</x:t>
+    <x:t>Payment Issue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00164</x:t>
   </x:si>
   <x:si>
     <x:t>Sophia</x:t>
@@ -403,10 +385,7 @@
     <x:t xml:space="preserve"> My printer isn't connecting to the Wi-Fi network.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Hardware Issue"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00075</x:t>
+    <x:t>CS2025_00165</x:t>
   </x:si>
   <x:si>
     <x:t>Tom</x:t>
@@ -418,10 +397,10 @@
     <x:t xml:space="preserve"> Is there a user manual for your latest product?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Product Support"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00076</x:t>
+    <x:t>Product Support.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00166</x:t>
   </x:si>
   <x:si>
     <x:t>Uma</x:t>
@@ -433,10 +412,10 @@
     <x:t xml:space="preserve"> The application freezes when I try to upload large files.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Performance Issue"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00077</x:t>
+    <x:t>Performance Issue.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00167</x:t>
   </x:si>
   <x:si>
     <x:t>Victor</x:t>
@@ -448,10 +427,7 @@
     <x:t xml:space="preserve"> I need assistance updating my payment method for my account.</x:t>
   </x:si>
   <x:si>
-    <x:t>Subscription Management</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00078</x:t>
+    <x:t>CS2025_00168</x:t>
   </x:si>
   <x:si>
     <x:t>Wendy</x:t>
@@ -463,10 +439,10 @@
     <x:t xml:space="preserve"> Do you provide training for your enterprise software?</x:t>
   </x:si>
   <x:si>
-    <x:t>Subcategory Suggestion: Training Services</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00079</x:t>
+    <x:t>Training Services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00169</x:t>
   </x:si>
   <x:si>
     <x:t>Xavier</x:t>
@@ -478,10 +454,10 @@
     <x:t xml:space="preserve"> I can't access my account because of a two-factor authentication issue.</x:t>
   </x:si>
   <x:si>
-    <x:t>"Account Access"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00080</x:t>
+    <x:t>Account Access.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00170</x:t>
   </x:si>
   <x:si>
     <x:t>Yolanda</x:t>
@@ -493,10 +469,10 @@
     <x:t xml:space="preserve"> How can I get a detailed breakdown of my charges for the last six months?</x:t>
   </x:si>
   <x:si>
-    <x:t>"Account Inquiries"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS2025_00081</x:t>
+    <x:t>Account Inquiries</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS2025_00171</x:t>
   </x:si>
   <x:si>
     <x:t>Zachary</x:t>
@@ -508,7 +484,7 @@
     <x:t xml:space="preserve"> Does your service offer multi - language support?</x:t>
   </x:si>
   <x:si>
-    <x:t>Subcategory Suggestion: Technical Support</x:t>
+    <x:t>Technical Support.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -859,7 +835,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G32"/>
+  <x:dimension ref="A1:G31"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1125,387 +1101,367 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="B14" s="0" t="s">
+      <x:c r="C14" s="0" t="s">
         <x:v>71</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>72</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
         <x:v>73</x:v>
-      </x:c>
-      <x:c r="G14" s="0" t="s">
-        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7">
       <x:c r="A15" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="B15" s="0" t="s">
+      <x:c r="C15" s="0" t="s">
         <x:v>76</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>77</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
         <x:v>78</x:v>
-      </x:c>
-      <x:c r="G15" s="0" t="s">
-        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:7">
       <x:c r="A16" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
         <x:v>80</x:v>
       </x:c>
-      <x:c r="B16" s="0" t="s">
+      <x:c r="C16" s="0" t="s">
         <x:v>81</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>82</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
         <x:v>83</x:v>
-      </x:c>
-      <x:c r="G16" s="0" t="s">
-        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
       <x:c r="A17" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="B17" s="0" t="s">
+      <x:c r="C17" s="0" t="s">
         <x:v>86</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>87</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
         <x:v>88</x:v>
-      </x:c>
-      <x:c r="G17" s="0" t="s">
-        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:7">
       <x:c r="A18" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="B18" s="0" t="s">
+      <x:c r="C18" s="0" t="s">
         <x:v>91</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>92</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
         <x:v>93</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:7">
       <x:c r="A19" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
         <x:v>95</x:v>
       </x:c>
-      <x:c r="B19" s="0" t="s">
+      <x:c r="C19" s="0" t="s">
         <x:v>96</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>97</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
         <x:v>98</x:v>
-      </x:c>
-      <x:c r="G19" s="0" t="s">
-        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:7">
       <x:c r="A20" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
         <x:v>100</x:v>
       </x:c>
-      <x:c r="B20" s="0" t="s">
+      <x:c r="C20" s="0" t="s">
         <x:v>101</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>102</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="s">
         <x:v>103</x:v>
-      </x:c>
-      <x:c r="G20" s="0" t="s">
-        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7">
       <x:c r="A21" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
-      <x:c r="B21" s="0" t="s">
+      <x:c r="C21" s="0" t="s">
         <x:v>106</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>107</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="s">
         <x:v>108</x:v>
-      </x:c>
-      <x:c r="G21" s="0" t="s">
-        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:7">
       <x:c r="A22" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
         <x:v>110</x:v>
       </x:c>
-      <x:c r="B22" s="0" t="s">
+      <x:c r="C22" s="0" t="s">
         <x:v>111</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>112</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
         <x:v>113</x:v>
-      </x:c>
-      <x:c r="G22" s="0" t="s">
-        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:7">
       <x:c r="A23" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
         <x:v>115</x:v>
       </x:c>
-      <x:c r="B23" s="0" t="s">
+      <x:c r="C23" s="0" t="s">
         <x:v>116</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="s">
-        <x:v>117</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="s">
         <x:v>118</x:v>
-      </x:c>
-      <x:c r="G23" s="0" t="s">
-        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:7">
       <x:c r="A24" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
         <x:v>120</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
+      <x:c r="C24" s="0" t="s">
         <x:v>121</x:v>
       </x:c>
-      <x:c r="C24" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="D24" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
         <x:v>122</x:v>
       </x:c>
-      <x:c r="E24" s="0" t="s">
-        <x:v>123</x:v>
-      </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:7">
       <x:c r="A25" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
         <x:v>125</x:v>
       </x:c>
-      <x:c r="B25" s="0" t="s">
+      <x:c r="D25" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
         <x:v>126</x:v>
       </x:c>
-      <x:c r="C25" s="0" t="s">
+      <x:c r="G25" s="0" t="s">
         <x:v>127</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E25" s="0" t="s">
-        <x:v>128</x:v>
-      </x:c>
-      <x:c r="G25" s="0" t="s">
-        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:7">
       <x:c r="A26" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="B26" s="0" t="s">
+      <x:c r="D26" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
         <x:v>131</x:v>
       </x:c>
-      <x:c r="C26" s="0" t="s">
+      <x:c r="G26" s="0" t="s">
         <x:v>132</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E26" s="0" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="G26" s="0" t="s">
-        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:7">
       <x:c r="A27" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
         <x:v>135</x:v>
       </x:c>
-      <x:c r="B27" s="0" t="s">
+      <x:c r="D27" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
         <x:v>136</x:v>
       </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>137</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E27" s="0" t="s">
-        <x:v>138</x:v>
-      </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:7">
       <x:c r="A28" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
         <x:v>140</x:v>
       </x:c>
-      <x:c r="B28" s="0" t="s">
+      <x:c r="G28" s="0" t="s">
         <x:v>141</x:v>
-      </x:c>
-      <x:c r="C28" s="0" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E28" s="0" t="s">
-        <x:v>143</x:v>
-      </x:c>
-      <x:c r="G28" s="0" t="s">
-        <x:v>144</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:7">
       <x:c r="A29" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
         <x:v>145</x:v>
       </x:c>
-      <x:c r="B29" s="0" t="s">
+      <x:c r="G29" s="0" t="s">
         <x:v>146</x:v>
-      </x:c>
-      <x:c r="C29" s="0" t="s">
-        <x:v>147</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E29" s="0" t="s">
-        <x:v>148</x:v>
-      </x:c>
-      <x:c r="G29" s="0" t="s">
-        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:7">
       <x:c r="A30" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
         <x:v>150</x:v>
       </x:c>
-      <x:c r="B30" s="0" t="s">
+      <x:c r="G30" s="0" t="s">
         <x:v>151</x:v>
-      </x:c>
-      <x:c r="C30" s="0" t="s">
-        <x:v>152</x:v>
-      </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E30" s="0" t="s">
-        <x:v>153</x:v>
-      </x:c>
-      <x:c r="G30" s="0" t="s">
-        <x:v>154</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:7">
       <x:c r="A31" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
         <x:v>155</x:v>
       </x:c>
-      <x:c r="B31" s="0" t="s">
+      <x:c r="G31" s="0" t="s">
         <x:v>156</x:v>
-      </x:c>
-      <x:c r="C31" s="0" t="s">
-        <x:v>157</x:v>
-      </x:c>
-      <x:c r="D31" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E31" s="0" t="s">
-        <x:v>158</x:v>
-      </x:c>
-      <x:c r="G31" s="0" t="s">
-        <x:v>159</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:7">
-      <x:c r="A32" s="0" t="s">
-        <x:v>160</x:v>
-      </x:c>
-      <x:c r="B32" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="C32" s="0" t="s">
-        <x:v>162</x:v>
-      </x:c>
-      <x:c r="D32" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E32" s="0" t="s">
-        <x:v>163</x:v>
-      </x:c>
-      <x:c r="G32" s="0" t="s">
-        <x:v>164</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>